<commit_message>
fixed some templates (e.g. referee name present instead of <referee>), added "yellow" highlight to sentences that should be checked (e.g. repetition of minutes and such)
</commit_message>
<xml_diff>
--- a/Databases/Templates GoalgetterLoss.xlsx
+++ b/Databases/Templates GoalgetterLoss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10412"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Syncmap\Promotie\PASS\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzo/Projects/PASS/Databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376116E9-5585-45AD-9B34-40AD11ED5921}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A1DEF-1C58-CA43-96F5-827EF6C08070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,13 +1148,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1166,10 +1178,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1179,9 +1192,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Neutrale" xfId="1" builtinId="28"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1197,7 +1212,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1520,16 +1535,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CS25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AZ13" sqref="AZ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="97" width="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97">
+    <row r="1" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:97">
+    <row r="2" spans="1:97" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1912,7 +1927,7 @@
       <c r="AY2" t="s">
         <v>76</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ2" s="5" t="s">
         <v>77</v>
       </c>
       <c r="BA2" t="s">
@@ -2042,7 +2057,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:97">
+    <row r="3" spans="1:97" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2118,7 +2133,7 @@
       <c r="AY3" t="s">
         <v>124</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="AZ3" s="5" t="s">
         <v>150</v>
       </c>
       <c r="BH3" t="s">
@@ -2191,7 +2206,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:97">
+    <row r="4" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2301,7 +2316,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:97">
+    <row r="5" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>351</v>
       </c>
@@ -2381,7 +2396,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:97">
+    <row r="6" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>268</v>
       </c>
@@ -2446,7 +2461,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:97">
+    <row r="7" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>269</v>
       </c>
@@ -2493,7 +2508,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:97">
+    <row r="8" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>270</v>
       </c>
@@ -2537,7 +2552,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:97">
+    <row r="9" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -2578,7 +2593,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:97">
+    <row r="10" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>188</v>
       </c>
@@ -2619,7 +2634,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:97">
+    <row r="11" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -2660,7 +2675,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:97">
+    <row r="12" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>272</v>
       </c>
@@ -2701,7 +2716,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:97">
+    <row r="13" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>276</v>
       </c>
@@ -2739,7 +2754,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:97">
+    <row r="14" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>277</v>
       </c>
@@ -2774,7 +2789,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:97">
+    <row r="15" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>281</v>
       </c>
@@ -2806,7 +2821,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:97">
+    <row r="16" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>282</v>
       </c>
@@ -2835,7 +2850,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:78">
+    <row r="17" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>286</v>
       </c>
@@ -2864,7 +2879,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:78">
+    <row r="18" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>287</v>
       </c>
@@ -2890,7 +2905,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:78">
+    <row r="19" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -2898,7 +2913,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:78">
+    <row r="20" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>294</v>
       </c>
@@ -2906,7 +2921,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:78">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>295</v>
       </c>
@@ -2914,22 +2929,22 @@
         <v>365</v>
       </c>
     </row>
-    <row r="22" spans="1:78">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="1:78">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="24" spans="1:78">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="25" spans="1:78">
+    <row r="25" spans="1:78" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>308</v>
       </c>
@@ -2947,9 +2962,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
@@ -2965,9 +2980,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
   </sheetData>

</xml_diff>